<commit_message>
add Csquares to VME polygon options map. Closes #3
</commit_message>
<xml_diff>
--- a/Output/MapLayerDesc.xlsx
+++ b/Output/MapLayerDesc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cefas-my.sharepoint.com/personal/anna_downie_cefas_co_uk/Documents/VME/ICES VME Benchmark/rmarkdown VMEs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neilm\Documents\projects\VME-Advice\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="8_{0C67439F-1C21-4420-8890-4FE16B91DC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AAF6903C-E191-4447-BAC4-155ED02BDAC2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AFB38D-A5B6-43A3-95C5-FE71B5948909}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{863AB745-BCE7-4B95-8481-8B52A9B598DC}"/>
   </bookViews>
@@ -21,22 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="61">
   <si>
     <t>Selectable layer</t>
   </si>
@@ -573,7 +563,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A5" sqref="A5:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -778,10 +768,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{536FB7B7-F14F-4571-841C-439237BA5B41}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -848,122 +838,144 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
         <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
         <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
         <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
         <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
         <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
         <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
         <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>47</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>